<commit_message>
Final version of the code
</commit_message>
<xml_diff>
--- a/Lines_data.xlsx
+++ b/Lines_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marta\Desktop\Sustainable Energy\OMPS\Project\optimization_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45F23D5-8E0A-47CB-A0CE-7E854EDFA520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41A770F-8F6E-4ACB-9118-2B74C7CEB0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +576,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>1.46E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E2">
         <v>175</v>
@@ -593,7 +593,7 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <v>0.2253</v>
+        <v>2E-3</v>
       </c>
       <c r="E3">
         <v>175</v>
@@ -610,7 +610,7 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <v>9.0700000000000003E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E4">
         <v>350</v>
@@ -627,7 +627,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>0.1356</v>
+        <v>2E-3</v>
       </c>
       <c r="E5">
         <v>175</v>
@@ -644,7 +644,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>0.20499999999999999</v>
+        <v>2E-3</v>
       </c>
       <c r="E6">
         <v>175</v>
@@ -661,7 +661,7 @@
         <v>9</v>
       </c>
       <c r="D7">
-        <v>0.12709999999999999</v>
+        <v>2E-3</v>
       </c>
       <c r="E7">
         <v>175</v>
@@ -678,7 +678,7 @@
         <v>24</v>
       </c>
       <c r="D8">
-        <v>8.4000000000000005E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E8">
         <v>400</v>
@@ -695,7 +695,7 @@
         <v>9</v>
       </c>
       <c r="D9">
-        <v>0.111</v>
+        <v>2E-3</v>
       </c>
       <c r="E9">
         <v>175</v>
@@ -712,7 +712,7 @@
         <v>10</v>
       </c>
       <c r="D10">
-        <v>9.4E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E10">
         <v>350</v>
@@ -729,7 +729,7 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>6.4199999999999993E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E11">
         <v>175</v>
@@ -746,7 +746,7 @@
         <v>8</v>
       </c>
       <c r="D12">
-        <v>6.5199999999999994E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E12">
         <v>350</v>
@@ -763,7 +763,7 @@
         <v>9</v>
       </c>
       <c r="D13">
-        <v>0.1762</v>
+        <v>2E-3</v>
       </c>
       <c r="E13">
         <v>175</v>
@@ -780,7 +780,7 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <v>0.1762</v>
+        <v>2E-3</v>
       </c>
       <c r="E14">
         <v>175</v>
@@ -797,7 +797,7 @@
         <v>11</v>
       </c>
       <c r="D15">
-        <v>8.4000000000000005E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E15">
         <v>400</v>
@@ -814,7 +814,7 @@
         <v>12</v>
       </c>
       <c r="D16">
-        <v>8.4000000000000005E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E16">
         <v>400</v>
@@ -831,7 +831,7 @@
         <v>11</v>
       </c>
       <c r="D17">
-        <v>8.4000000000000005E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E17">
         <v>400</v>
@@ -848,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="D18">
-        <v>8.4000000000000005E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E18">
         <v>400</v>
@@ -865,7 +865,7 @@
         <v>13</v>
       </c>
       <c r="D19">
-        <v>4.8800000000000003E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E19">
         <v>500</v>
@@ -882,7 +882,7 @@
         <v>14</v>
       </c>
       <c r="D20">
-        <v>4.2599999999999999E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E20">
         <v>500</v>
@@ -899,7 +899,7 @@
         <v>13</v>
       </c>
       <c r="D21">
-        <v>4.8800000000000003E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E21">
         <v>500</v>
@@ -916,7 +916,7 @@
         <v>23</v>
       </c>
       <c r="D22">
-        <v>9.8500000000000004E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E22">
         <v>500</v>
@@ -933,7 +933,7 @@
         <v>23</v>
       </c>
       <c r="D23">
-        <v>8.8400000000000006E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E23">
         <v>500</v>
@@ -950,7 +950,7 @@
         <v>16</v>
       </c>
       <c r="D24">
-        <v>5.9400000000000001E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E24">
         <v>500</v>
@@ -967,7 +967,7 @@
         <v>16</v>
       </c>
       <c r="D25">
-        <v>1.72E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E25">
         <v>500</v>
@@ -984,7 +984,7 @@
         <v>21</v>
       </c>
       <c r="D26">
-        <v>2.4899999999999999E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E26">
         <v>1000</v>
@@ -1001,7 +1001,7 @@
         <v>24</v>
       </c>
       <c r="D27">
-        <v>5.2900000000000003E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E27">
         <v>500</v>
@@ -1018,7 +1018,7 @@
         <v>17</v>
       </c>
       <c r="D28">
-        <v>2.63E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E28">
         <v>500</v>
@@ -1035,7 +1035,7 @@
         <v>19</v>
       </c>
       <c r="D29">
-        <v>2.3400000000000001E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E29">
         <v>500</v>
@@ -1052,7 +1052,7 @@
         <v>18</v>
       </c>
       <c r="D30">
-        <v>1.43E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E30">
         <v>500</v>
@@ -1069,7 +1069,7 @@
         <v>22</v>
       </c>
       <c r="D31">
-        <v>0.1069</v>
+        <v>2E-3</v>
       </c>
       <c r="E31">
         <v>500</v>
@@ -1086,7 +1086,7 @@
         <v>21</v>
       </c>
       <c r="D32">
-        <v>1.32E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E32">
         <v>1000</v>
@@ -1103,7 +1103,7 @@
         <v>20</v>
       </c>
       <c r="D33">
-        <v>2.0299999999999999E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E33">
         <v>1000</v>
@@ -1120,7 +1120,7 @@
         <v>23</v>
       </c>
       <c r="D34">
-        <v>1.12E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E34">
         <v>1000</v>
@@ -1137,7 +1137,7 @@
         <v>22</v>
       </c>
       <c r="D35">
-        <v>6.9199999999999998E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="E35">
         <v>500</v>
@@ -1150,9 +1150,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1300,26 +1303,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{702244EF-09E4-4287-A309-D47118C6EA68}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1E3775B-1FA2-47C8-9DD7-1455AFF9DA69}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="59a1f2c9-9aa0-4700-bb29-973d29195b9e"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1343,9 +1335,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1E3775B-1FA2-47C8-9DD7-1455AFF9DA69}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{702244EF-09E4-4287-A309-D47118C6EA68}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="59a1f2c9-9aa0-4700-bb29-973d29195b9e"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>